<commit_message>
ajout des compétences mobiliser et du tableau de synthese completer
</commit_message>
<xml_diff>
--- a/portfolio/pdf/Tableau_de_synthèse.xlsx
+++ b/portfolio/pdf/Tableau_de_synthèse.xlsx
@@ -1,87 +1,81 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <workbookPr/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
-    <t xml:space="preserve">BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SESSION 2022</t>
+    <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
+  </si>
+  <si>
+    <t>SESSION 2022</t>
   </si>
   <si>
     <t xml:space="preserve">Tableau de synthèse des réalisations professionnelles </t>
   </si>
   <si>
-    <t xml:space="preserve">NOM et prénom : </t>
+    <t>NOM et prénom : Titouan Le Brun A Vali Patel</t>
   </si>
   <si>
     <t xml:space="preserve">N° candidat : </t>
   </si>
   <si>
-    <t xml:space="preserve">Centre de formation :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Option :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">▢ SISR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">▢ SLAM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresse URL du portfolio :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compétences mises en œuvre
+    <t>Centre de formation :</t>
+  </si>
+  <si>
+    <t>Option :</t>
+  </si>
+  <si>
+    <t>▢ SISR</t>
+  </si>
+  <si>
+    <t>X SLAM</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : titouanlebrunavalipatel.github.io/portfolio</t>
+  </si>
+  <si>
+    <t>Compétences mises en œuvre
 Réalisations professionnelles
 (intitulé et liste des documents et productions associés)</t>
   </si>
   <si>
-    <t xml:space="preserve">Période (sous la forme du JJ/MM/AA au JJ/MM/AA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gérer le patrimoine informatique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Répondre aux incidents et aux demandes d’assistance et d’évolution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Développer la présence en ligne de l’organisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Travailler en mode projet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mettre à disposition des utilisateurs un service informatique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organiser son développement professionnel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">▸Recenser et identifier les ressources numériques 
+    <t>Période (sous la forme du JJ/MM/AA au JJ/MM/AA)</t>
+  </si>
+  <si>
+    <t>Gérer le patrimoine informatique</t>
+  </si>
+  <si>
+    <t>Répondre aux incidents et aux demandes d’assistance et d’évolution</t>
+  </si>
+  <si>
+    <t>Développer la présence en ligne de l’organisation</t>
+  </si>
+  <si>
+    <t>Travailler en mode projet</t>
+  </si>
+  <si>
+    <t>Mettre à disposition des utilisateurs un service informatique</t>
+  </si>
+  <si>
+    <t>Organiser son développement professionnel</t>
+  </si>
+  <si>
+    <t>▸Recenser et identifier les ressources numériques 
 ▸Exploiter des référentiels, normes et standards adoptés par le prestataire informatique
 ▸Mettre en place et vérifier les niveaux d’habilitation associés à un service
 ▸Vérifier les conditions de la continuité d’un service informatique
@@ -89,27 +83,27 @@
 ▸Vérifier le respect des règles d’utilisation des ressources numériques</t>
   </si>
   <si>
-    <t xml:space="preserve">▸Collecter, suivre et orienter des demandes 
+    <t>▸Collecter, suivre et orienter des demandes 
 ▸Traiter des demandes concernant les services réseau et système, applicatifs
 ▸Traiter des demandes concernant les applications</t>
   </si>
   <si>
-    <t xml:space="preserve">▸Participer à la valorisation de l’image de l’organisation sur les médias numériques en tenant compte du cadre juridique et des enjeux économiques
+    <t>▸Participer à la valorisation de l’image de l’organisation sur les médias numériques en tenant compte du cadre juridique et des enjeux économiques
 ▸Référencer les services en ligne de l’organisation et mesurer leur visibilité.
 ▸Participer à l’évolution d’un site Web exploitant les données de l’organisation.</t>
   </si>
   <si>
-    <t xml:space="preserve">▸Analyser les objectifs et les modalités d’organisation d’un projet
+    <t>▸Analyser les objectifs et les modalités d’organisation d’un projet
 ▸Planifier les activités
 ▸Évaluer les indicateurs de suivi d’un projet et analyser les écarts</t>
   </si>
   <si>
-    <t xml:space="preserve">▸Réaliser les tests d’intégration et d’acceptation d’un service
+    <t>▸Réaliser les tests d’intégration et d’acceptation d’un service
 ▸Déployer un service
 ▸Accompagner les utilisateurs dans la mise en place d’un service</t>
   </si>
   <si>
-    <t xml:space="preserve">▸Mettre en place son environnement d’apprentissage personnel
+    <t>▸Mettre en place son environnement d’apprentissage personnel
 ▸Mettre en œuvre des outils et stratégies de veille informationnelle
 ▸Gérer son identité professionnelle
 ▸Développer son projet professionnel</t>
@@ -119,61 +113,61 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Projet la Fleur Gestion de panier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13/02/22 au 13/05/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kayak'mor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12/01/22 au 12/02/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x</t>
+    <t>Projet la Fleur Gestion de panier</t>
+  </si>
+  <si>
+    <t>13/02/22 au 13/05/22</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Kayak'mor</t>
+  </si>
+  <si>
+    <t>12/01/22 au 12/02/22</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
   <si>
     <t xml:space="preserve">Stage France Poultry – Châteaulin </t>
   </si>
   <si>
-    <t xml:space="preserve">29/05/22 au 03/07/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Réalisations en milieu professionnel en cours de première année</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stage France Poultry – Châteaulin : Mission 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30/05/22 au 01/06/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stage France Poultry – Châteaulin : Mission 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03/06/22 au 10/06/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stage France Poultry – Châteaulin : Mission 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11/06/22 au 14/06/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stage France Poultry – Châteaulin : Mission 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15/06/22 au 01/06/22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Réalisations en milieu professionnel en cours de seconde année</t>
+    <t>29/05/22 au 03/07/22</t>
+  </si>
+  <si>
+    <t>Réalisations en milieu professionnel en cours de première année</t>
+  </si>
+  <si>
+    <t>Stage France Poultry – Châteaulin : Mission 1</t>
+  </si>
+  <si>
+    <t>30/05/22 au 01/06/22</t>
+  </si>
+  <si>
+    <t>Stage France Poultry – Châteaulin : Mission 2</t>
+  </si>
+  <si>
+    <t>03/06/22 au 10/06/22</t>
+  </si>
+  <si>
+    <t>Stage France Poultry – Châteaulin : Mission 3</t>
+  </si>
+  <si>
+    <t>Stage France Poultry – Châteaulin : Mission 4</t>
+  </si>
+  <si>
+    <t>15/06/22 au 01/06/22</t>
+  </si>
+  <si>
+    <t>Réalisations en milieu professionnel en cours de seconde année</t>
+  </si>
+  <si>
+    <t>11/06/2022 au 14/06/2022</t>
+  </si>
+  <si>
+    <t>XX</t>
   </si>
 </sst>
 </file>
@@ -193,63 +187,48 @@
     </font>
     <font>
       <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <family val="0"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="20"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <i val="true"/>
+      <b/>
+      <i/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -268,15 +247,35 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -290,14 +289,14 @@
     </fill>
   </fills>
   <borders count="20">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF4A452A"/>
       </left>
@@ -310,9 +309,8 @@
       <bottom style="thin">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -325,9 +323,8 @@
       <bottom style="thin">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF4A452A"/>
       </left>
@@ -340,9 +337,8 @@
       <bottom style="thin">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -353,9 +349,8 @@
       <bottom style="thin">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -364,9 +359,8 @@
       <bottom style="thin">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right style="medium">
         <color rgb="FF4A452A"/>
@@ -377,9 +371,8 @@
       <bottom style="thin">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF4A452A"/>
       </left>
@@ -392,9 +385,8 @@
       <bottom style="medium">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="true">
+    <border diagonalDown="1">
       <left style="medium">
         <color rgb="FF4A452A"/>
       </left>
@@ -409,7 +401,7 @@
         <color rgb="FF4A452A"/>
       </diagonal>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -422,9 +414,8 @@
       <bottom style="medium">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -437,9 +428,8 @@
       <bottom style="thin">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -450,9 +440,8 @@
         <color rgb="FF4A452A"/>
       </top>
       <bottom/>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -463,9 +452,8 @@
         <color rgb="FF4A452A"/>
       </top>
       <bottom/>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF4A452A"/>
       </left>
@@ -478,9 +466,8 @@
       <bottom style="thin">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -493,9 +480,8 @@
       <bottom style="thin">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -508,9 +494,8 @@
       <bottom style="thin">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF4A452A"/>
       </left>
@@ -523,9 +508,8 @@
       <bottom style="thin">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="medium">
         <color rgb="FF4A452A"/>
       </left>
@@ -538,9 +522,8 @@
       <bottom style="medium">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -553,9 +536,8 @@
       <bottom style="medium">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left style="thin">
         <color rgb="FF4A452A"/>
       </left>
@@ -568,276 +550,626 @@
       <bottom style="medium">
         <color rgb="FF4A452A"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="21">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
+      <alignment/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellXfs count="45">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
     <cellStyle name="Euro" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF4A452A"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="004A452A"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{e71f3f7a-f24d-464b-8705-c04ea9834c5e}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ81"/>
+  <dimension ref="A1:AQ35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A13">
+      <selection pane="topLeft" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="63.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="18.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="9" style="2" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="44" style="1" width="10.85"/>
+    <col min="1" max="1" width="63.142857142857146" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.285714285714285" style="1" customWidth="1"/>
+    <col min="3" max="4" width="18.571428571428573" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.142857142857142" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.857142857142858" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.142857142857142" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.285714285714285" style="1" customWidth="1"/>
+    <col min="9" max="43" width="11.428571428571429" style="2" customWidth="1"/>
+    <col min="44" max="1025" width="10.857142857142858" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:8" ht="39.95" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -851,7 +1183,7 @@
       </c>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" customFormat="false" ht="41.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:8" ht="41.1" customHeight="1" thickBot="1">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -863,7 +1195,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:13" ht="39.95" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -880,7 +1212,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:8" ht="39.95" customHeight="1">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -898,7 +1230,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:8" ht="39.95" customHeight="1" thickBot="1">
       <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
@@ -910,7 +1242,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="90" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:8" ht="90" customHeight="1" thickBot="1">
       <c r="A6" s="11" t="s">
         <v>10</v>
       </c>
@@ -936,7 +1268,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" s="17" customFormat="true" ht="324.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:43" s="17" customFormat="1" ht="324.95" customHeight="1" thickBot="1">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="15" t="s">
@@ -993,7 +1325,7 @@
       <c r="AP7" s="2"/>
       <c r="AQ7" s="2"/>
     </row>
-    <row r="8" s="17" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:43" s="17" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="18" t="s">
         <v>24</v>
       </c>
@@ -1040,7 +1372,7 @@
       <c r="AP8" s="2"/>
       <c r="AQ8" s="2"/>
     </row>
-    <row r="9" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>25</v>
       </c>
@@ -1093,7 +1425,7 @@
       <c r="AP9" s="2"/>
       <c r="AQ9" s="2"/>
     </row>
-    <row r="10" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>28</v>
       </c>
@@ -1148,7 +1480,7 @@
       <c r="AP10" s="2"/>
       <c r="AQ10" s="2"/>
     </row>
-    <row r="11" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>31</v>
       </c>
@@ -1203,7 +1535,7 @@
       <c r="AP11" s="2"/>
       <c r="AQ11" s="2"/>
     </row>
-    <row r="12" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A12" s="19"/>
       <c r="B12" s="20"/>
       <c r="C12" s="22"/>
@@ -1248,7 +1580,7 @@
       <c r="AP12" s="2"/>
       <c r="AQ12" s="2"/>
     </row>
-    <row r="13" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A13" s="19"/>
       <c r="B13" s="20"/>
       <c r="C13" s="22"/>
@@ -1293,7 +1625,7 @@
       <c r="AP13" s="2"/>
       <c r="AQ13" s="2"/>
     </row>
-    <row r="14" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A14" s="19"/>
       <c r="B14" s="20"/>
       <c r="C14" s="22"/>
@@ -1338,7 +1670,7 @@
       <c r="AP14" s="2"/>
       <c r="AQ14" s="2"/>
     </row>
-    <row r="15" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A15" s="19"/>
       <c r="B15" s="20"/>
       <c r="C15" s="22"/>
@@ -1383,7 +1715,7 @@
       <c r="AP15" s="2"/>
       <c r="AQ15" s="2"/>
     </row>
-    <row r="16" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A16" s="19"/>
       <c r="B16" s="20"/>
       <c r="C16" s="22"/>
@@ -1428,7 +1760,7 @@
       <c r="AP16" s="2"/>
       <c r="AQ16" s="2"/>
     </row>
-    <row r="17" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="22"/>
@@ -1473,7 +1805,7 @@
       <c r="AP17" s="2"/>
       <c r="AQ17" s="2"/>
     </row>
-    <row r="18" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A18" s="19"/>
       <c r="B18" s="20"/>
       <c r="C18" s="22"/>
@@ -1518,7 +1850,7 @@
       <c r="AP18" s="2"/>
       <c r="AQ18" s="2"/>
     </row>
-    <row r="19" s="17" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:43" s="17" customFormat="1" ht="18">
       <c r="A19" s="26" t="s">
         <v>33</v>
       </c>
@@ -1565,29 +1897,29 @@
       <c r="AP19" s="2"/>
       <c r="AQ19" s="2"/>
     </row>
-    <row r="20" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="27" t="s">
+    <row r="20" spans="1:43" s="17" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A20" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="36" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
@@ -1616,31 +1948,31 @@
       <c r="AP20" s="2"/>
       <c r="AQ20" s="2"/>
     </row>
-    <row r="21" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="27" t="s">
+    <row r="21" spans="1:43" s="17" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A21" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22" t="s">
+      <c r="C21" s="38"/>
+      <c r="D21" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
@@ -1669,31 +2001,31 @@
       <c r="AP21" s="2"/>
       <c r="AQ21" s="2"/>
     </row>
-    <row r="22" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="27" t="s">
+    <row r="22" spans="1:43" s="17" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A22" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="B22" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22" t="s">
+      <c r="B22" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22" t="s">
+      <c r="F22" s="38"/>
+      <c r="G22" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="23"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="44"/>
+      <c r="J22" s="44"/>
+      <c r="K22" s="44"/>
+      <c r="L22" s="44"/>
+      <c r="M22" s="44"/>
+      <c r="N22" s="44"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="44"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
@@ -1722,33 +2054,33 @@
       <c r="AP22" s="2"/>
       <c r="AQ22" s="2"/>
     </row>
-    <row r="23" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27" t="s">
+    <row r="23" spans="1:43" s="17" customFormat="1" ht="39.75" customHeight="1">
+      <c r="A23" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="G23" s="22" t="s">
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="23"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="44"/>
+      <c r="M23" s="44"/>
+      <c r="N23" s="44"/>
+      <c r="O23" s="44"/>
+      <c r="P23" s="44"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
@@ -1777,7 +2109,7 @@
       <c r="AP23" s="2"/>
       <c r="AQ23" s="2"/>
     </row>
-    <row r="24" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A24" s="19"/>
       <c r="B24" s="20"/>
       <c r="C24" s="22"/>
@@ -1822,7 +2154,7 @@
       <c r="AP24" s="2"/>
       <c r="AQ24" s="2"/>
     </row>
-    <row r="25" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A25" s="19"/>
       <c r="B25" s="20"/>
       <c r="C25" s="22"/>
@@ -1867,7 +2199,7 @@
       <c r="AP25" s="2"/>
       <c r="AQ25" s="2"/>
     </row>
-    <row r="26" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A26" s="19"/>
       <c r="B26" s="20"/>
       <c r="C26" s="22"/>
@@ -1912,9 +2244,9 @@
       <c r="AP26" s="2"/>
       <c r="AQ26" s="2"/>
     </row>
-    <row r="27" s="17" customFormat="true" ht="18" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:43" s="17" customFormat="1" ht="18">
       <c r="A27" s="26" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B27" s="26"/>
       <c r="C27" s="26"/>
@@ -1959,7 +2291,7 @@
       <c r="AP27" s="2"/>
       <c r="AQ27" s="2"/>
     </row>
-    <row r="28" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A28" s="19"/>
       <c r="B28" s="20"/>
       <c r="C28" s="22"/>
@@ -2004,7 +2336,7 @@
       <c r="AP28" s="2"/>
       <c r="AQ28" s="2"/>
     </row>
-    <row r="29" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A29" s="19"/>
       <c r="B29" s="20"/>
       <c r="C29" s="22"/>
@@ -2049,7 +2381,7 @@
       <c r="AP29" s="2"/>
       <c r="AQ29" s="2"/>
     </row>
-    <row r="30" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A30" s="19"/>
       <c r="B30" s="20"/>
       <c r="C30" s="22"/>
@@ -2094,7 +2426,7 @@
       <c r="AP30" s="2"/>
       <c r="AQ30" s="2"/>
     </row>
-    <row r="31" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A31" s="19"/>
       <c r="B31" s="20"/>
       <c r="C31" s="22"/>
@@ -2139,7 +2471,7 @@
       <c r="AP31" s="2"/>
       <c r="AQ31" s="2"/>
     </row>
-    <row r="32" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A32" s="19"/>
       <c r="B32" s="20"/>
       <c r="C32" s="22"/>
@@ -2184,7 +2516,7 @@
       <c r="AP32" s="2"/>
       <c r="AQ32" s="2"/>
     </row>
-    <row r="33" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1">
       <c r="A33" s="19"/>
       <c r="B33" s="20"/>
       <c r="C33" s="22"/>
@@ -2229,7 +2561,7 @@
       <c r="AP33" s="2"/>
       <c r="AQ33" s="2"/>
     </row>
-    <row r="34" s="17" customFormat="true" ht="39.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:43" s="17" customFormat="1" ht="39.95" customHeight="1" thickBot="1">
       <c r="A34" s="28"/>
       <c r="B34" s="29"/>
       <c r="C34" s="30"/>
@@ -2274,7 +2606,7 @@
       <c r="AP34" s="2"/>
       <c r="AQ34" s="2"/>
     </row>
-    <row r="35" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:43" s="17" customFormat="1" ht="15">
       <c r="A35" s="32"/>
       <c r="B35" s="33"/>
       <c r="C35" s="34"/>
@@ -2319,52 +2651,52 @@
       <c r="AP35" s="2"/>
       <c r="AQ35" s="2"/>
     </row>
-    <row r="36" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" s="2" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" s="2" customFormat="1" ht="12.75"/>
+    <row r="37" s="2" customFormat="1" ht="12.75"/>
+    <row r="38" s="2" customFormat="1" ht="12.75"/>
+    <row r="39" s="2" customFormat="1" ht="12.75"/>
+    <row r="40" s="2" customFormat="1" ht="12.75"/>
+    <row r="41" s="2" customFormat="1" ht="12.75"/>
+    <row r="42" s="2" customFormat="1" ht="12.75"/>
+    <row r="43" s="2" customFormat="1" ht="12.75"/>
+    <row r="44" s="2" customFormat="1" ht="12.75"/>
+    <row r="45" s="2" customFormat="1" ht="12.75"/>
+    <row r="46" s="2" customFormat="1" ht="12.75"/>
+    <row r="47" s="2" customFormat="1" ht="12.75"/>
+    <row r="48" s="2" customFormat="1" ht="12.75"/>
+    <row r="49" s="2" customFormat="1" ht="12.75"/>
+    <row r="50" s="2" customFormat="1" ht="12.75"/>
+    <row r="51" s="2" customFormat="1" ht="12.75"/>
+    <row r="52" s="2" customFormat="1" ht="12.75"/>
+    <row r="53" s="2" customFormat="1" ht="12.75"/>
+    <row r="54" s="2" customFormat="1" ht="12.75"/>
+    <row r="55" s="2" customFormat="1" ht="12.75"/>
+    <row r="56" s="2" customFormat="1" ht="12.75"/>
+    <row r="57" s="2" customFormat="1" ht="12.75"/>
+    <row r="58" s="2" customFormat="1" ht="12.75"/>
+    <row r="59" s="2" customFormat="1" ht="12.75"/>
+    <row r="60" s="2" customFormat="1" ht="12.75"/>
+    <row r="61" s="2" customFormat="1" ht="12.75"/>
+    <row r="62" s="2" customFormat="1" ht="12.75"/>
+    <row r="63" s="2" customFormat="1" ht="12.75"/>
+    <row r="64" s="2" customFormat="1" ht="12.75"/>
+    <row r="65" s="2" customFormat="1" ht="12.75"/>
+    <row r="66" s="2" customFormat="1" ht="12.75"/>
+    <row r="67" s="2" customFormat="1" ht="12.75"/>
+    <row r="68" s="2" customFormat="1" ht="12.75"/>
+    <row r="69" s="2" customFormat="1" ht="12.75"/>
+    <row r="70" s="2" customFormat="1" ht="12.75"/>
+    <row r="71" s="2" customFormat="1" ht="12.75"/>
+    <row r="72" s="2" customFormat="1" ht="12.75"/>
+    <row r="73" s="2" customFormat="1" ht="12.75"/>
+    <row r="74" s="2" customFormat="1" ht="12.75"/>
+    <row r="75" s="2" customFormat="1" ht="12.75"/>
+    <row r="76" s="2" customFormat="1" ht="12.75"/>
+    <row r="77" s="2" customFormat="1" ht="12.75"/>
+    <row r="78" s="2" customFormat="1" ht="12.75"/>
+    <row r="79" s="2" customFormat="1" ht="12.75"/>
+    <row r="80" s="2" customFormat="1" ht="12.75"/>
+    <row r="81" s="2" customFormat="1" ht="12.75"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="A1:F1"/>
@@ -2380,12 +2712,8 @@
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A27:H27"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.196527777777778" right="0.196527777777778" top="0.196527777777778" bottom="0.196527777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup horizontalDpi="300" verticalDpi="300" orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rajout de mon stage chez Verlingue Quimper
</commit_message>
<xml_diff>
--- a/portfolio/pdf/Tableau_de_synthèse.xlsx
+++ b/portfolio/pdf/Tableau_de_synthèse.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\titou\OneDrive\Bureau\Titouan\TitouanLeBrunAValiPatel.github.io\portfolio\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1474D15-D163-406C-A06E-480F7A557AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6AAC16-EEF7-4E92-9EFC-A37304E8C188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -137,12 +137,6 @@
     <t>x</t>
   </si>
   <si>
-    <t xml:space="preserve">Stage France Poultry – Châteaulin </t>
-  </si>
-  <si>
-    <t>29/05/22 au 03/07/22</t>
-  </si>
-  <si>
     <t>Réalisations en milieu professionnel en cours de première année</t>
   </si>
   <si>
@@ -179,10 +173,37 @@
     <t>03/01/23 au 16/01/23</t>
   </si>
   <si>
-    <t>Stage Verlingue - Quimper (Recenser et identifier les ressources numériques)</t>
-  </si>
-  <si>
-    <t>Stage Verlingue - Quimper (Déployer un service)</t>
+    <t>09/01/23 au 11/01/23</t>
+  </si>
+  <si>
+    <t>Stage Verlingue - Quimper (Prendre connaissance des enjeux et des documentations techniques)</t>
+  </si>
+  <si>
+    <t>Stage Verlingue - Quimper (Préparer son poste de travail)</t>
+  </si>
+  <si>
+    <t>Stage Verlingue - Quimper  (Création de nouvelles méthodes dans la class Melusine)</t>
+  </si>
+  <si>
+    <t>12/01/23 au 30/01/23</t>
+  </si>
+  <si>
+    <t>Stage Verlingue - Quimper (Gestion des erreurs)</t>
+  </si>
+  <si>
+    <t>31/01/23 au 08/02/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stage Verlingue - Quimper (Profil Linkedin) </t>
+  </si>
+  <si>
+    <t>08/02/23 au 10/02/23</t>
+  </si>
+  <si>
+    <t>Tuleap campus - Appli Frais</t>
+  </si>
+  <si>
+    <t>22/11/22 au 20/04/23</t>
   </si>
 </sst>
 </file>
@@ -586,35 +607,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -711,6 +705,36 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1100,141 +1124,141 @@
   </sheetPr>
   <dimension ref="A1:AMK81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.1796875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="36.26953125" style="10" customWidth="1"/>
-    <col min="3" max="4" width="18.54296875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="16.81640625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="18.1796875" style="10" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="63.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.26953125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="18.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" style="1" customWidth="1"/>
     <col min="9" max="43" width="11.453125" customWidth="1"/>
-    <col min="44" max="1025" width="10.81640625" style="10" customWidth="1"/>
+    <col min="44" max="1025" width="10.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="9"/>
+      <c r="H1" s="34"/>
     </row>
     <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="7" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="11" t="s">
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="10" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="16" t="s">
+    <row r="7" spans="1:43" s="1" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="40"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
       <c r="I7"/>
@@ -1273,17 +1297,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:43" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1320,23 +1344,23 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+    <row r="9" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="22"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="13"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1373,23 +1397,23 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+    <row r="10" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="23" t="s">
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="21"/>
-      <c r="H10" s="24" t="s">
+      <c r="G10" s="12"/>
+      <c r="H10" s="15" t="s">
         <v>30</v>
       </c>
       <c r="I10"/>
@@ -1428,25 +1452,27 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="23" t="s">
+    <row r="11" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="23" t="s">
+      <c r="D11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="23" t="s">
+      <c r="E11" s="14"/>
+      <c r="F11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="G11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H11" s="13"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1483,15 +1509,15 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
+    <row r="12" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1528,15 +1554,15 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22"/>
+    <row r="13" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1573,15 +1599,15 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="22"/>
+    <row r="14" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="13"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1618,15 +1644,15 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="22"/>
+    <row r="15" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="13"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1663,15 +1689,15 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22"/>
+    <row r="16" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1708,15 +1734,15 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="22"/>
+    <row r="17" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="13"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1753,15 +1779,15 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="22"/>
+    <row r="18" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1798,17 +1824,17 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+    <row r="19" spans="1:43" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1845,29 +1871,29 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="10" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="34" t="s">
+    <row r="20" spans="1:43" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-      <c r="L20" s="37"/>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37"/>
-      <c r="O20" s="37"/>
-      <c r="P20" s="37"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
       <c r="Q20"/>
       <c r="R20"/>
       <c r="S20"/>
@@ -1896,31 +1922,31 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="10" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35" t="s">
+    <row r="21" spans="1:43" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="E21" s="35" t="s">
+      <c r="E21" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-      <c r="L21" s="37"/>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37"/>
-      <c r="O21" s="37"/>
-      <c r="P21" s="37"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
       <c r="Q21"/>
       <c r="R21"/>
       <c r="S21"/>
@@ -1949,31 +1975,31 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="10" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B22" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35" t="s">
+    <row r="22" spans="1:43" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35" t="s">
+      <c r="F22" s="26"/>
+      <c r="G22" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H22" s="40"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
       <c r="Q22"/>
       <c r="R22"/>
       <c r="S22"/>
@@ -2002,33 +2028,33 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="10" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B23" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="35" t="s">
+    <row r="23" spans="1:43" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="35" t="s">
+      <c r="D23" s="26"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H23" s="40"/>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
       <c r="Q23"/>
       <c r="R23"/>
       <c r="S23"/>
@@ -2057,15 +2083,15 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="22"/>
+    <row r="24" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="13"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2102,15 +2128,15 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="22"/>
+    <row r="25" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="13"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2147,15 +2173,15 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
+    <row r="26" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="13"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2192,17 +2218,17 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+    <row r="27" spans="1:43" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2239,21 +2265,21 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B28" s="42" t="s">
+    <row r="28" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="B28" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="22"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="13"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2290,19 +2316,21 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" s="19"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21" t="s">
+    <row r="29" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H29" s="22"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="13"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2339,15 +2367,21 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="22"/>
+    <row r="30" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="13"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2384,15 +2418,21 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18"/>
-      <c r="B31" s="19"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="22"/>
+    <row r="31" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H31" s="13"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2429,15 +2469,21 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="22"/>
+    <row r="32" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2474,15 +2520,15 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="22"/>
+    <row r="33" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="13"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2519,15 +2565,15 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="10" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="27"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="28"/>
+    <row r="34" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="16"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="19"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2564,15 +2610,15 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="10" customFormat="1" ht="14" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
+    <row r="35" spans="1:43" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>

</xml_diff>

<commit_message>
ajout du tableau de synthèe en dynamique
</commit_message>
<xml_diff>
--- a/portfolio/pdf/Tableau_de_synthèse.xlsx
+++ b/portfolio/pdf/Tableau_de_synthèse.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Documents\TitouanLeBrunAValiPatel.github.io\portfolio\pdf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temporaire\TitouanLeBrunAValiPatel.github.io\portfolio\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11A4D6A-C66E-4B2E-9E78-FDE31F692416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="25425" windowHeight="16305" tabRatio="500"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -210,11 +211,17 @@
   <si>
     <t>27/02/23 au 17/03/23</t>
   </si>
+  <si>
+    <t>Gestion d'incident - GLPI</t>
+  </si>
+  <si>
+    <t>22/03/23 au 29/03/23</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* \-??\ [$€-1]_-"/>
   </numFmts>
@@ -714,6 +721,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -732,18 +748,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Euro" xfId="1"/>
+    <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1123,80 +1130,80 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AMK81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="18.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="1" customWidth="1"/>
-    <col min="9" max="43" width="11.42578125" customWidth="1"/>
-    <col min="44" max="1025" width="10.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="63.1796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.26953125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="18.54296875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.81640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" style="1" customWidth="1"/>
+    <col min="9" max="43" width="11.453125" customWidth="1"/>
+    <col min="44" max="1025" width="10.81640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="41"/>
-    </row>
-    <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="H1" s="35"/>
+    </row>
+    <row r="2" spans="1:43" ht="41.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-    </row>
-    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+    </row>
+    <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="43" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
+    <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1207,23 +1214,23 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="37" t="s">
+    <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-    </row>
-    <row r="6" spans="1:43" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+    </row>
+    <row r="6" spans="1:43" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="42" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1245,9 +1252,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:43" s="1" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38"/>
-      <c r="B7" s="39"/>
+    <row r="7" spans="1:43" s="1" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="41"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="7" t="s">
         <v>18</v>
       </c>
@@ -1302,17 +1309,17 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40" t="s">
+    <row r="8" spans="1:43" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="40"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1349,7 +1356,7 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>25</v>
       </c>
@@ -1402,7 +1409,7 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>28</v>
       </c>
@@ -1457,7 +1464,7 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>52</v>
       </c>
@@ -1514,7 +1521,7 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>54</v>
       </c>
@@ -1565,10 +1572,16 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="12"/>
+    <row r="13" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
@@ -1610,7 +1623,7 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="12"/>
@@ -1655,7 +1668,7 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="10"/>
       <c r="C15" s="12"/>
@@ -1700,7 +1713,7 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="10"/>
       <c r="C16" s="12"/>
@@ -1745,7 +1758,7 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="10"/>
       <c r="C17" s="12"/>
@@ -1790,7 +1803,7 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="10"/>
       <c r="C18" s="12"/>
@@ -1835,17 +1848,17 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
+    <row r="19" spans="1:43" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A19" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1882,7 +1895,7 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:43" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>32</v>
       </c>
@@ -1933,7 +1946,7 @@
       <c r="AP20"/>
       <c r="AQ20"/>
     </row>
-    <row r="21" spans="1:43" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:43" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="29" t="s">
         <v>34</v>
       </c>
@@ -1986,7 +1999,7 @@
       <c r="AP21"/>
       <c r="AQ21"/>
     </row>
-    <row r="22" spans="1:43" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:43" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29" t="s">
         <v>36</v>
       </c>
@@ -2039,7 +2052,7 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:43" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="29" t="s">
         <v>37</v>
       </c>
@@ -2094,7 +2107,7 @@
       <c r="AP23"/>
       <c r="AQ23"/>
     </row>
-    <row r="24" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="10"/>
       <c r="C24" s="12"/>
@@ -2139,7 +2152,7 @@
       <c r="AP24"/>
       <c r="AQ24"/>
     </row>
-    <row r="25" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9"/>
       <c r="B25" s="10"/>
       <c r="C25" s="12"/>
@@ -2184,7 +2197,7 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="10"/>
       <c r="C26" s="12"/>
@@ -2229,17 +2242,17 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="35" t="s">
+    <row r="27" spans="1:43" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A27" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="35"/>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
+      <c r="B27" s="38"/>
+      <c r="C27" s="38"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="38"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2276,7 +2289,7 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>44</v>
       </c>
@@ -2327,7 +2340,7 @@
       <c r="AP28"/>
       <c r="AQ28"/>
     </row>
-    <row r="29" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>45</v>
       </c>
@@ -2378,7 +2391,7 @@
       <c r="AP29"/>
       <c r="AQ29"/>
     </row>
-    <row r="30" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>46</v>
       </c>
@@ -2429,7 +2442,7 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>48</v>
       </c>
@@ -2480,7 +2493,7 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>50</v>
       </c>
@@ -2531,7 +2544,7 @@
       <c r="AP32"/>
       <c r="AQ32"/>
     </row>
-    <row r="33" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9"/>
       <c r="B33" s="10"/>
       <c r="C33" s="12"/>
@@ -2576,7 +2589,7 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="17"/>
       <c r="C34" s="18"/>
@@ -2621,7 +2634,7 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:43" s="1" customFormat="1" ht="14" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
       <c r="B35" s="21"/>
       <c r="C35" s="22"/>
@@ -2666,59 +2679,54 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="A4:E4"/>
@@ -2726,6 +2734,11 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.196527777777778" right="0.196527777777778" top="0.196527777777778" bottom="0.196527777777778" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
ajout d'animation + modification code couleur
</commit_message>
<xml_diff>
--- a/portfolio/pdf/Tableau_de_synthèse.xlsx
+++ b/portfolio/pdf/Tableau_de_synthèse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temporaire\TitouanLeBrunAValiPatel.github.io\portfolio\pdf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11A4D6A-C66E-4B2E-9E78-FDE31F692416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE03FE6-0DCB-4B70-8881-E2FA73087305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,9 +200,6 @@
     <t>08/02/23 au 10/02/23</t>
   </si>
   <si>
-    <t>Tuleap campus - Appli Frais</t>
-  </si>
-  <si>
     <t>22/11/22 au 20/04/23</t>
   </si>
   <si>
@@ -216,6 +213,9 @@
   </si>
   <si>
     <t>22/03/23 au 29/03/23</t>
+  </si>
+  <si>
+    <t>Tuleap campus - Appli Frais (Gestion des fiches de frais)</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1137,7 @@
   <dimension ref="A1:AMK81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1466,10 +1466,10 @@
     </row>
     <row r="11" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="33" t="s">
         <v>52</v>
-      </c>
-      <c r="B11" s="33" t="s">
-        <v>53</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>27</v>
@@ -1523,10 +1523,10 @@
     </row>
     <row r="12" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="33" t="s">
         <v>54</v>
-      </c>
-      <c r="B12" s="33" t="s">
-        <v>55</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>27</v>
@@ -1574,10 +1574,10 @@
     </row>
     <row r="13" spans="1:43" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="33" t="s">
         <v>56</v>
-      </c>
-      <c r="B13" s="33" t="s">
-        <v>57</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>27</v>
@@ -2742,6 +2742,6 @@
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.196527777777778" right="0.196527777777778" top="0.196527777777778" bottom="0.196527777777778" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" scale="48" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="49" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>